<commit_message>
Move the list of skills inside the character instead of player
</commit_message>
<xml_diff>
--- a/doc/RadMudEditor.xlsx
+++ b/doc/RadMudEditor.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RaceBaseSkill" sheetId="8" r:id="rId1"/>
     <sheet name="RaceBaseAbility" sheetId="9" r:id="rId2"/>
     <sheet name="SkillManager" sheetId="7" r:id="rId3"/>
-    <sheet name="Variables" sheetId="6" r:id="rId4"/>
+    <sheet name="SkillAreas" sheetId="10" r:id="rId4"/>
+    <sheet name="Variables" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Ability">Variables!$C$2:$C$6</definedName>
@@ -803,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -2828,7 +2829,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3908,10 +3909,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Move modifiers inside the enumerators folder
</commit_message>
<xml_diff>
--- a/doc/RadMudEditor.xlsx
+++ b/doc/RadMudEditor.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RaceBaseSkill" sheetId="8" r:id="rId1"/>
     <sheet name="RaceBaseAbility" sheetId="9" r:id="rId2"/>
     <sheet name="SkillManager" sheetId="7" r:id="rId3"/>
-    <sheet name="SkillAreas" sheetId="10" r:id="rId4"/>
-    <sheet name="Variables" sheetId="6" r:id="rId5"/>
+    <sheet name="Variables" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Ability">Variables!$C$2:$C$6</definedName>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="116">
   <si>
     <t>Athletics</t>
   </si>
@@ -804,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -2826,10 +2825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2845,11 +2844,16 @@
     <col min="9" max="9" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="7"/>
+    <col min="12" max="12" width="2.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>81</v>
       </c>
@@ -2864,8 +2868,15 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="M1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
@@ -2897,267 +2908,423 @@
       <c r="K2" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="5"/>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7">
+        <f>VLOOKUP(A3,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <f>VLOOKUP(B3,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <f>VLOOKUP(C3,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <f>VLOOKUP(D3,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <f>VLOOKUP(E3,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M16" si="0">CONCATENATE("""", G3, """")</f>
+        <v>"1"</v>
+      </c>
+      <c r="N3" s="7" t="str">
+        <f t="shared" ref="N3:N16" si="1">CONCATENATE("""", H3, """")</f>
+        <v>"0"</v>
+      </c>
+      <c r="O3" s="7" t="str">
+        <f t="shared" ref="O3:O16" si="2">CONCATENATE("""", I3, """")</f>
+        <v>"0"</v>
+      </c>
+      <c r="P3" s="7" t="str">
+        <f t="shared" ref="P3:P16" si="3">CONCATENATE("""", J3, """")</f>
+        <v>"1"</v>
+      </c>
+      <c r="Q3" s="7" t="str">
+        <f t="shared" ref="Q3:Q16" si="4">CONCATENATE("""", K3, """")</f>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="7">
+        <f>VLOOKUP(A4,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="7">
+        <f>VLOOKUP(B4,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <f>VLOOKUP(C4,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <f>VLOOKUP(D4,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="K4" s="7">
+        <f>VLOOKUP(E4,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"2"</v>
+      </c>
+      <c r="N4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"5"</v>
+      </c>
+      <c r="Q4" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="7">
+        <f>VLOOKUP(A5,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="7">
+        <f>VLOOKUP(B5,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <f>VLOOKUP(C5,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="J5" s="7">
+        <f>VLOOKUP(D5,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <f>VLOOKUP(E5,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"4"</v>
+      </c>
+      <c r="N5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O5" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"5"</v>
+      </c>
+      <c r="P5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q5" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A3,Variables!$E$2:$F$34,2,FALSE), """")</f>
+      <c r="G6" s="7">
+        <f>VLOOKUP(A6,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H6" s="7">
+        <f>VLOOKUP(B6,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <f>VLOOKUP(C6,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <f>VLOOKUP(D6,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <f>VLOOKUP(E6,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>"7"</v>
       </c>
-      <c r="H3" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B3,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I3" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C3,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J3" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D3,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K3" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E3,Variables!$M$2:$N$34,2,FALSE), """")</f>
+      <c r="N6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q6" s="7" t="str">
+        <f t="shared" si="4"/>
         <v>"1"</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A4,Variables!$E$2:$F$34,2,FALSE), """")</f>
+      <c r="G7" s="7">
+        <f>VLOOKUP(A7,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H7" s="7">
+        <f>VLOOKUP(B7,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <f>VLOOKUP(C7,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <f>VLOOKUP(D7,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <f>VLOOKUP(E7,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>"7"</v>
       </c>
-      <c r="H4" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B4,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C4,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J4" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D4,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K4" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E4,Variables!$M$2:$N$34,2,FALSE), """")</f>
+      <c r="N7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O7" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q7" s="7" t="str">
+        <f t="shared" si="4"/>
         <v>"2"</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A5,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>"1"</v>
-      </c>
-      <c r="H5" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B5,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I5" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C5,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J5" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D5,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"1"</v>
-      </c>
-      <c r="K5" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E5,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A6,Variables!$E$2:$F$36,2,FALSE), """")</f>
-        <v>"34"</v>
-      </c>
-      <c r="H6" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B6,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I6" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C6,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J6" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D6,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"3"</v>
-      </c>
-      <c r="K6" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E6,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A7,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>"2"</v>
-      </c>
-      <c r="H7" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B7,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I7" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C7,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J7" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D7,Variables!$K$2:$L$34,2,FALSE), """")</f>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="7">
+        <f>VLOOKUP(A8,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="7">
+        <f>VLOOKUP(B8,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <f>VLOOKUP(C8,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <f>VLOOKUP(D8,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <f>VLOOKUP(E8,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10"</v>
+      </c>
+      <c r="N8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O8" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q8" s="7" t="str">
+        <f t="shared" si="4"/>
         <v>"5"</v>
       </c>
-      <c r="K7" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E7,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A8,Variables!$E$2:$F$36,2,FALSE), """")</f>
-        <v>"35"</v>
-      </c>
-      <c r="H8" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B8,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I8" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C8,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J8" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D8,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"7"</v>
-      </c>
-      <c r="K8" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E8,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A9,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>"4"</v>
-      </c>
-      <c r="H9" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B9,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I9" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C9,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"5"</v>
-      </c>
-      <c r="J9" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D9,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K9" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E9,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7">
+        <f>VLOOKUP(A9,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="H9" s="7">
+        <f>VLOOKUP(B9,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <f>VLOOKUP(C9,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <f>VLOOKUP(D9,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <f>VLOOKUP(E9,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10"</v>
+      </c>
+      <c r="N9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O9" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q9" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"6"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
@@ -3173,30 +3340,50 @@
       <c r="E10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A10,Variables!$E$2:$F$34,2,FALSE), """")</f>
+      <c r="G10" s="7">
+        <f>VLOOKUP(A10,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="H10" s="7">
+        <f>VLOOKUP(B10,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <f>VLOOKUP(C10,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="J10" s="7">
+        <f>VLOOKUP(D10,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <f>VLOOKUP(E10,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>"14"</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B10,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I10" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C10,Variables!$I$2:$J$34,2,FALSE), """")</f>
+      <c r="N10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O10" s="7" t="str">
+        <f t="shared" si="2"/>
         <v>"7"</v>
       </c>
-      <c r="J10" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D10,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K10" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E10,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q10" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>46</v>
@@ -3205,35 +3392,55 @@
         <v>46</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A11,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>"10"</v>
-      </c>
-      <c r="H11" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B11,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I11" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C11,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J11" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D11,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K11" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E11,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"5"</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="G11" s="7">
+        <f>VLOOKUP(A11,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="H11" s="7">
+        <f>VLOOKUP(B11,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f>VLOOKUP(C11,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f>VLOOKUP(D11,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K11" s="7">
+        <f>VLOOKUP(E11,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"34"</v>
+      </c>
+      <c r="N11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O11" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"3"</v>
+      </c>
+      <c r="Q11" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>46</v>
@@ -3242,33 +3449,53 @@
         <v>46</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(A12,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>"10"</v>
-      </c>
-      <c r="H12" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B12,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I12" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C12,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J12" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D12,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K12" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E12,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"6"</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="G12" s="7">
+        <f>VLOOKUP(A12,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="H12" s="7">
+        <f>VLOOKUP(B12,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <f>VLOOKUP(C12,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <f>VLOOKUP(D12,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="K12" s="7">
+        <f>VLOOKUP(E12,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"35"</v>
+      </c>
+      <c r="N12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O12" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"7"</v>
+      </c>
+      <c r="Q12" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
         <v>46</v>
       </c>
@@ -3282,27 +3509,47 @@
         <v>46</v>
       </c>
       <c r="G13" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A13,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H13" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B13,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I13" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C13,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J13" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D13,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K13" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E13,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A13,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H13" s="7">
+        <f>VLOOKUP(B13,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <f>VLOOKUP(C13,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <f>VLOOKUP(D13,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <f>VLOOKUP(E13,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q13" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
         <v>46</v>
       </c>
@@ -3316,27 +3563,47 @@
         <v>46</v>
       </c>
       <c r="G14" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A14,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B14,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I14" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C14,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J14" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D14,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K14" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E14,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A14,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="7">
+        <f>VLOOKUP(B14,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <f>VLOOKUP(C14,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <f>VLOOKUP(D14,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
+        <f>VLOOKUP(E14,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q14" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
         <v>46</v>
       </c>
@@ -3350,27 +3617,47 @@
         <v>46</v>
       </c>
       <c r="G15" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A15,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H15" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B15,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I15" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C15,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J15" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D15,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K15" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E15,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A15,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="7">
+        <f>VLOOKUP(B15,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <f>VLOOKUP(C15,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <f>VLOOKUP(D15,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <f>VLOOKUP(E15,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q15" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
         <v>46</v>
       </c>
@@ -3384,27 +3671,47 @@
         <v>46</v>
       </c>
       <c r="G16" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A16,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H16" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B16,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I16" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C16,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J16" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D16,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K16" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E16,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A16,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" s="7">
+        <f>VLOOKUP(B16,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <f>VLOOKUP(C16,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <f>VLOOKUP(D16,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <f>VLOOKUP(E16,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"0"</v>
+      </c>
+      <c r="O16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"0"</v>
+      </c>
+      <c r="P16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q16" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
         <v>46</v>
       </c>
@@ -3418,27 +3725,47 @@
         <v>46</v>
       </c>
       <c r="G17" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A17,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H17" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B17,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I17" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C17,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J17" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D17,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K17" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E17,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A17,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" s="7">
+        <f>VLOOKUP(B17,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <f>VLOOKUP(C17,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <f>VLOOKUP(D17,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <f>VLOOKUP(E17,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="7" t="e">
+        <f t="shared" ref="M17:M30" si="5">CONCATENATE("""", G17, """")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N17" s="7" t="str">
+        <f t="shared" ref="N17:N30" si="6">CONCATENATE("""", H17, """")</f>
+        <v>"0"</v>
+      </c>
+      <c r="O17" s="7" t="str">
+        <f t="shared" ref="O17:O30" si="7">CONCATENATE("""", I17, """")</f>
+        <v>"0"</v>
+      </c>
+      <c r="P17" s="7" t="str">
+        <f t="shared" ref="P17:P30" si="8">CONCATENATE("""", J17, """")</f>
+        <v>"0"</v>
+      </c>
+      <c r="Q17" s="7" t="str">
+        <f t="shared" ref="Q17:Q30" si="9">CONCATENATE("""", K17, """")</f>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>46</v>
       </c>
@@ -3452,27 +3779,47 @@
         <v>46</v>
       </c>
       <c r="G18" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A18,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H18" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B18,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I18" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C18,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J18" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D18,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K18" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E18,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A18,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H18" s="7">
+        <f>VLOOKUP(B18,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <f>VLOOKUP(C18,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <f>VLOOKUP(D18,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <f>VLOOKUP(E18,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N18" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O18" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P18" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q18" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
@@ -3486,27 +3833,47 @@
         <v>46</v>
       </c>
       <c r="G19" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A19,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H19" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B19,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I19" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C19,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J19" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D19,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K19" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E19,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A19,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H19" s="7">
+        <f>VLOOKUP(B19,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
+        <f>VLOOKUP(C19,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <f>VLOOKUP(D19,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
+        <f>VLOOKUP(E19,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N19" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O19" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P19" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>46</v>
       </c>
@@ -3520,27 +3887,47 @@
         <v>46</v>
       </c>
       <c r="G20" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A20,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H20" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B20,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I20" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C20,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J20" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D20,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K20" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E20,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A20,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H20" s="7">
+        <f>VLOOKUP(B20,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <f>VLOOKUP(C20,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <f>VLOOKUP(D20,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <f>VLOOKUP(E20,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N20" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O20" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P20" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q20" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>46</v>
       </c>
@@ -3554,27 +3941,47 @@
         <v>46</v>
       </c>
       <c r="G21" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A21,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H21" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B21,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I21" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C21,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J21" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D21,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K21" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E21,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A21,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H21" s="7">
+        <f>VLOOKUP(B21,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="7">
+        <f>VLOOKUP(C21,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="7">
+        <f>VLOOKUP(D21,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <f>VLOOKUP(E21,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N21" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O21" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P21" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q21" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>46</v>
       </c>
@@ -3588,27 +3995,47 @@
         <v>46</v>
       </c>
       <c r="G22" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A22,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B22,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I22" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C22,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J22" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D22,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K22" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E22,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A22,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H22" s="7">
+        <f>VLOOKUP(B22,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="7">
+        <f>VLOOKUP(C22,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="7">
+        <f>VLOOKUP(D22,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="7">
+        <f>VLOOKUP(E22,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N22" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O22" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P22" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q22" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>46</v>
       </c>
@@ -3622,27 +4049,47 @@
         <v>46</v>
       </c>
       <c r="G23" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A23,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H23" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B23,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I23" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C23,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J23" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D23,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K23" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E23,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A23,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H23" s="7">
+        <f>VLOOKUP(B23,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
+        <f>VLOOKUP(C23,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="7">
+        <f>VLOOKUP(D23,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
+        <f>VLOOKUP(E23,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N23" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O23" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P23" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q23" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
         <v>46</v>
       </c>
@@ -3656,27 +4103,47 @@
         <v>46</v>
       </c>
       <c r="G24" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A24,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H24" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B24,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I24" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C24,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J24" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D24,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K24" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E24,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A24,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H24" s="7">
+        <f>VLOOKUP(B24,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="7">
+        <f>VLOOKUP(C24,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="7">
+        <f>VLOOKUP(D24,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="7">
+        <f>VLOOKUP(E24,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N24" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O24" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P24" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q24" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>46</v>
       </c>
@@ -3690,27 +4157,47 @@
         <v>46</v>
       </c>
       <c r="G25" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A25,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H25" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B25,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I25" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C25,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J25" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D25,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K25" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E25,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A25,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H25" s="7">
+        <f>VLOOKUP(B25,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="7">
+        <f>VLOOKUP(C25,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="7">
+        <f>VLOOKUP(D25,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
+        <f>VLOOKUP(E25,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O25" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P25" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q25" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
         <v>46</v>
       </c>
@@ -3724,27 +4211,47 @@
         <v>46</v>
       </c>
       <c r="G26" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A26,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H26" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B26,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I26" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C26,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J26" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D26,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K26" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E26,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A26,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H26" s="7">
+        <f>VLOOKUP(B26,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
+        <f>VLOOKUP(C26,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <f>VLOOKUP(D26,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
+        <f>VLOOKUP(E26,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N26" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O26" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P26" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q26" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>46</v>
       </c>
@@ -3758,27 +4265,47 @@
         <v>46</v>
       </c>
       <c r="G27" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A27,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H27" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B27,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I27" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C27,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J27" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D27,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K27" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E27,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A27,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H27" s="7">
+        <f>VLOOKUP(B27,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
+        <f>VLOOKUP(C27,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <f>VLOOKUP(D27,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
+        <f>VLOOKUP(E27,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N27" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O27" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P27" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q27" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="9" t="s">
         <v>46</v>
       </c>
@@ -3792,27 +4319,47 @@
         <v>46</v>
       </c>
       <c r="G28" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A28,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H28" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B28,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I28" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C28,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J28" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D28,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K28" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E28,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A28,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H28" s="7">
+        <f>VLOOKUP(B28,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <f>VLOOKUP(C28,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <f>VLOOKUP(D28,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <f>VLOOKUP(E28,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N28" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O28" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P28" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q28" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="9" t="s">
         <v>46</v>
       </c>
@@ -3826,27 +4373,47 @@
         <v>46</v>
       </c>
       <c r="G29" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A29,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H29" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B29,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I29" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C29,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J29" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D29,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K29" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E29,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(A29,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H29" s="7">
+        <f>VLOOKUP(B29,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="7">
+        <f>VLOOKUP(C29,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="7">
+        <f>VLOOKUP(D29,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <f>VLOOKUP(E29,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N29" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O29" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P29" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q29" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
         <v>46</v>
       </c>
@@ -3860,30 +4427,494 @@
         <v>46</v>
       </c>
       <c r="G30" s="7" t="e">
-        <f>CONCATENATE("""", VLOOKUP(A30,Variables!$E$2:$F$34,2,FALSE), """")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H30" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(B30,Variables!$G$2:$H$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="I30" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(C30,Variables!$I$2:$J$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="J30" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(D30,Variables!$K$2:$L$34,2,FALSE), """")</f>
-        <v>"0"</v>
-      </c>
-      <c r="K30" s="7" t="str">
-        <f>CONCATENATE("""", VLOOKUP(E30,Variables!$M$2:$N$34,2,FALSE), """")</f>
-        <v>"0"</v>
+        <f>VLOOKUP(A30,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H30" s="7">
+        <f>VLOOKUP(B30,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="7">
+        <f>VLOOKUP(C30,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="7">
+        <f>VLOOKUP(D30,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="7">
+        <f>VLOOKUP(E30,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N30" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0"</v>
+      </c>
+      <c r="O30" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0"</v>
+      </c>
+      <c r="P30" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>"0"</v>
+      </c>
+      <c r="Q30" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>"0"</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G31" s="7" t="e">
+        <f>VLOOKUP(A31,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H31" s="7" t="e">
+        <f>VLOOKUP(B31,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I31" s="7" t="e">
+        <f>VLOOKUP(C31,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J31" s="7" t="e">
+        <f>VLOOKUP(D31,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K31" s="7" t="e">
+        <f>VLOOKUP(E31,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G32" s="7" t="e">
+        <f>VLOOKUP(A32,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H32" s="7" t="e">
+        <f>VLOOKUP(B32,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I32" s="7" t="e">
+        <f>VLOOKUP(C32,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J32" s="7" t="e">
+        <f>VLOOKUP(D32,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K32" s="7" t="e">
+        <f>VLOOKUP(E32,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G33" s="7" t="e">
+        <f>VLOOKUP(A33,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H33" s="7" t="e">
+        <f>VLOOKUP(B33,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I33" s="7" t="e">
+        <f>VLOOKUP(C33,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J33" s="7" t="e">
+        <f>VLOOKUP(D33,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K33" s="7" t="e">
+        <f>VLOOKUP(E33,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G34" s="7" t="e">
+        <f>VLOOKUP(A34,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H34" s="7" t="e">
+        <f>VLOOKUP(B34,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I34" s="7" t="e">
+        <f>VLOOKUP(C34,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J34" s="7" t="e">
+        <f>VLOOKUP(D34,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K34" s="7" t="e">
+        <f>VLOOKUP(E34,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G35" s="7" t="e">
+        <f>VLOOKUP(A35,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H35" s="7" t="e">
+        <f>VLOOKUP(B35,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I35" s="7" t="e">
+        <f>VLOOKUP(C35,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J35" s="7" t="e">
+        <f>VLOOKUP(D35,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K35" s="7" t="e">
+        <f>VLOOKUP(E35,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G36" s="7" t="e">
+        <f>VLOOKUP(A36,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H36" s="7" t="e">
+        <f>VLOOKUP(B36,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I36" s="7" t="e">
+        <f>VLOOKUP(C36,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J36" s="7" t="e">
+        <f>VLOOKUP(D36,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K36" s="7" t="e">
+        <f>VLOOKUP(E36,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G37" s="7" t="e">
+        <f>VLOOKUP(A37,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H37" s="7" t="e">
+        <f>VLOOKUP(B37,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I37" s="7" t="e">
+        <f>VLOOKUP(C37,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J37" s="7" t="e">
+        <f>VLOOKUP(D37,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K37" s="7" t="e">
+        <f>VLOOKUP(E37,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G38" s="7" t="e">
+        <f>VLOOKUP(A38,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H38" s="7" t="e">
+        <f>VLOOKUP(B38,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I38" s="7" t="e">
+        <f>VLOOKUP(C38,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J38" s="7" t="e">
+        <f>VLOOKUP(D38,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K38" s="7" t="e">
+        <f>VLOOKUP(E38,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G39" s="7" t="e">
+        <f>VLOOKUP(A39,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H39" s="7" t="e">
+        <f>VLOOKUP(B39,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I39" s="7" t="e">
+        <f>VLOOKUP(C39,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J39" s="7" t="e">
+        <f>VLOOKUP(D39,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K39" s="7" t="e">
+        <f>VLOOKUP(E39,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G40" s="7" t="e">
+        <f>VLOOKUP(A40,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H40" s="7" t="e">
+        <f>VLOOKUP(B40,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I40" s="7" t="e">
+        <f>VLOOKUP(C40,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J40" s="7" t="e">
+        <f>VLOOKUP(D40,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K40" s="7" t="e">
+        <f>VLOOKUP(E40,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G41" s="7" t="e">
+        <f>VLOOKUP(A41,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H41" s="7" t="e">
+        <f>VLOOKUP(B41,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I41" s="7" t="e">
+        <f>VLOOKUP(C41,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J41" s="7" t="e">
+        <f>VLOOKUP(D41,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K41" s="7" t="e">
+        <f>VLOOKUP(E41,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G42" s="7" t="e">
+        <f>VLOOKUP(A42,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H42" s="7" t="e">
+        <f>VLOOKUP(B42,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I42" s="7" t="e">
+        <f>VLOOKUP(C42,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J42" s="7" t="e">
+        <f>VLOOKUP(D42,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K42" s="7" t="e">
+        <f>VLOOKUP(E42,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G43" s="7" t="e">
+        <f>VLOOKUP(A43,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H43" s="7" t="e">
+        <f>VLOOKUP(B43,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I43" s="7" t="e">
+        <f>VLOOKUP(C43,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J43" s="7" t="e">
+        <f>VLOOKUP(D43,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K43" s="7" t="e">
+        <f>VLOOKUP(E43,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G44" s="7" t="e">
+        <f>VLOOKUP(A44,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H44" s="7" t="e">
+        <f>VLOOKUP(B44,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I44" s="7" t="e">
+        <f>VLOOKUP(C44,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J44" s="7" t="e">
+        <f>VLOOKUP(D44,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K44" s="7" t="e">
+        <f>VLOOKUP(E44,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G45" s="7" t="e">
+        <f>VLOOKUP(A45,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H45" s="7" t="e">
+        <f>VLOOKUP(B45,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I45" s="7" t="e">
+        <f>VLOOKUP(C45,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J45" s="7" t="e">
+        <f>VLOOKUP(D45,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K45" s="7" t="e">
+        <f>VLOOKUP(E45,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G46" s="7" t="e">
+        <f>VLOOKUP(A46,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H46" s="7" t="e">
+        <f>VLOOKUP(B46,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I46" s="7" t="e">
+        <f>VLOOKUP(C46,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J46" s="7" t="e">
+        <f>VLOOKUP(D46,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K46" s="7" t="e">
+        <f>VLOOKUP(E46,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G47" s="7" t="e">
+        <f>VLOOKUP(A47,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H47" s="7" t="e">
+        <f>VLOOKUP(B47,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I47" s="7" t="e">
+        <f>VLOOKUP(C47,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J47" s="7" t="e">
+        <f>VLOOKUP(D47,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K47" s="7" t="e">
+        <f>VLOOKUP(E47,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G48" s="7" t="e">
+        <f>VLOOKUP(A48,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H48" s="7" t="e">
+        <f>VLOOKUP(B48,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I48" s="7" t="e">
+        <f>VLOOKUP(C48,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J48" s="7" t="e">
+        <f>VLOOKUP(D48,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K48" s="7" t="e">
+        <f>VLOOKUP(E48,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G49" s="7" t="e">
+        <f>VLOOKUP(A49,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H49" s="7" t="e">
+        <f>VLOOKUP(B49,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I49" s="7" t="e">
+        <f>VLOOKUP(C49,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J49" s="7" t="e">
+        <f>VLOOKUP(D49,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K49" s="7" t="e">
+        <f>VLOOKUP(E49,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G50" s="7" t="e">
+        <f>VLOOKUP(A50,Variables!$E$2:$F$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H50" s="7" t="e">
+        <f>VLOOKUP(B50,Variables!$G$2:$H$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I50" s="7" t="e">
+        <f>VLOOKUP(C50,Variables!$I$2:$J$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J50" s="7" t="e">
+        <f>VLOOKUP(D50,Variables!$K$2:$L$50,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K50" s="7" t="e">
+        <f>VLOOKUP(E50,Variables!$M$2:$N$50,2,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <sortState ref="A3:Q16">
+    <sortCondition ref="G3:G16"/>
+  </sortState>
+  <mergeCells count="3">
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Skills" sqref="A3:A30">
@@ -3909,24 +4940,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:R16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implement automatic skill unlock
</commit_message>
<xml_diff>
--- a/doc/RadMudEditor.xlsx
+++ b/doc/RadMudEditor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RaceBaseSkill" sheetId="8" r:id="rId1"/>
@@ -2068,15 +2068,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2084,6 +2075,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4590,7 +4590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
@@ -4632,60 +4632,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="33" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="33" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="36" t="s">
         <v>556</v>
       </c>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="33" t="s">
+      <c r="P1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="36" t="s">
         <v>556</v>
       </c>
-      <c r="S1" s="35"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="33" t="s">
+      <c r="S1" s="37"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="36" t="s">
         <v>557</v>
       </c>
-      <c r="V1" s="34"/>
-      <c r="W1" s="33" t="s">
+      <c r="V1" s="38"/>
+      <c r="W1" s="36" t="s">
         <v>557</v>
       </c>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="33" t="s">
+      <c r="X1" s="38"/>
+      <c r="Y1" s="36" t="s">
         <v>558</v>
       </c>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="36" t="s">
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="33" t="s">
         <v>558</v>
       </c>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="33" t="s">
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="33" t="s">
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="35"/>
+      <c r="AH1" s="37"/>
     </row>
     <row r="2" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -4895,11 +4895,11 @@
         <v>110</v>
       </c>
       <c r="AG3" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE3,ProductionList,0), 1)</f>
+        <f t="shared" ref="AG3:AG50" si="8">INDEX(ProductionListVnum, MATCH(AE3,ProductionList,0), 1)</f>
         <v>1</v>
       </c>
       <c r="AH3" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF3,Knowledge,0), 2)</f>
+        <f t="shared" ref="AH3:AH50" si="9">INDEX(KnowledgeVnum, MATCH(AF3,Knowledge,0), 2)</f>
         <v>17</v>
       </c>
     </row>
@@ -4924,7 +4924,7 @@
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19">
-        <f t="shared" ref="H4:H50" si="8">A4</f>
+        <f t="shared" ref="H4:H50" si="10">A4</f>
         <v>2</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -4997,7 +4997,7 @@
         <v>5</v>
       </c>
       <c r="AD4" s="20">
-        <f t="shared" ref="AD4:AD50" si="9">AA4</f>
+        <f t="shared" ref="AD4:AD50" si="11">AA4</f>
         <v>1</v>
       </c>
       <c r="AE4" s="11" t="s">
@@ -5007,11 +5007,11 @@
         <v>110</v>
       </c>
       <c r="AG4" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE4,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AH4" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF4,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
     </row>
@@ -5038,7 +5038,7 @@
         <v>489</v>
       </c>
       <c r="H5" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -5111,7 +5111,7 @@
         <v>2</v>
       </c>
       <c r="AD5" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AE5" s="11" t="s">
@@ -5121,11 +5121,11 @@
         <v>102</v>
       </c>
       <c r="AG5" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE5,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AH5" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF5,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
     </row>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -5223,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="AD6" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE6" s="11" t="s">
@@ -5233,11 +5233,11 @@
         <v>111</v>
       </c>
       <c r="AG6" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE6,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AH6" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF6,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
     </row>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="I7" s="11" t="s">
@@ -5335,7 +5335,7 @@
         <v>6</v>
       </c>
       <c r="AD7" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE7" s="11" t="s">
@@ -5345,11 +5345,11 @@
         <v>111</v>
       </c>
       <c r="AG7" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE7,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AH7" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF7,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
     </row>
@@ -5376,7 +5376,7 @@
         <v>490</v>
       </c>
       <c r="H8" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -5449,7 +5449,7 @@
         <v>4</v>
       </c>
       <c r="AD8" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE8" s="11" t="s">
@@ -5459,11 +5459,11 @@
         <v>102</v>
       </c>
       <c r="AG8" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE8,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AH8" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF8,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
     </row>
@@ -5490,7 +5490,7 @@
         <v>489</v>
       </c>
       <c r="H9" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="I9" s="11" t="s">
@@ -5563,7 +5563,7 @@
         <v>3</v>
       </c>
       <c r="AD9" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE9" s="11" t="s">
@@ -5573,11 +5573,11 @@
         <v>102</v>
       </c>
       <c r="AG9" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE9,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AH9" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF9,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
     </row>
@@ -5604,7 +5604,7 @@
         <v>490</v>
       </c>
       <c r="H10" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="I10" s="11" t="s">
@@ -5677,7 +5677,7 @@
         <v>3</v>
       </c>
       <c r="AD10" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="AE10" s="11" t="s">
@@ -5687,11 +5687,11 @@
         <v>102</v>
       </c>
       <c r="AG10" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE10,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AH10" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF10,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
     </row>
@@ -5716,7 +5716,7 @@
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="I11" s="11" t="s">
@@ -5789,7 +5789,7 @@
         <v>3</v>
       </c>
       <c r="AD11" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AE11" s="11" t="s">
@@ -5799,11 +5799,11 @@
         <v>112</v>
       </c>
       <c r="AG11" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE11,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AH11" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF11,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
@@ -5828,7 +5828,7 @@
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="I12" s="11" t="s">
@@ -5901,7 +5901,7 @@
         <v>5</v>
       </c>
       <c r="AD12" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE12" s="11" t="s">
@@ -5911,11 +5911,11 @@
         <v>112</v>
       </c>
       <c r="AG12" s="25">
-        <f>INDEX(ProductionListVnum, MATCH(AE12,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AH12" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF12,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
@@ -5930,7 +5930,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="20"/>
       <c r="H13" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="I13" s="11"/>
@@ -5989,7 +5989,7 @@
         <v>12</v>
       </c>
       <c r="AD13" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE13" s="19"/>
@@ -5997,11 +5997,11 @@
         <v>39</v>
       </c>
       <c r="AG13" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE13,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH13" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF13,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6016,7 +6016,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="20"/>
       <c r="H14" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="I14" s="11"/>
@@ -6075,7 +6075,7 @@
         <v>11</v>
       </c>
       <c r="AD14" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AE14" s="19"/>
@@ -6083,11 +6083,11 @@
         <v>39</v>
       </c>
       <c r="AG14" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE14,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH14" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF14,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6102,7 +6102,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="20"/>
       <c r="H15" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="I15" s="11"/>
@@ -6155,7 +6155,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD15" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE15" s="19"/>
@@ -6163,11 +6163,11 @@
         <v>39</v>
       </c>
       <c r="AG15" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE15,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH15" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF15,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6182,7 +6182,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="20"/>
       <c r="H16" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="I16" s="11"/>
@@ -6235,7 +6235,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD16" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE16" s="19"/>
@@ -6243,11 +6243,11 @@
         <v>39</v>
       </c>
       <c r="AG16" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE16,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH16" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF16,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6262,7 +6262,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="20"/>
       <c r="H17" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="I17" s="11"/>
@@ -6315,7 +6315,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD17" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE17" s="19"/>
@@ -6323,11 +6323,11 @@
         <v>39</v>
       </c>
       <c r="AG17" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE17,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH17" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF17,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6342,7 +6342,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="20"/>
       <c r="H18" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="I18" s="11"/>
@@ -6395,7 +6395,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD18" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE18" s="19"/>
@@ -6403,11 +6403,11 @@
         <v>39</v>
       </c>
       <c r="AG18" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE18,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH18" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF18,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6422,7 +6422,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="20"/>
       <c r="H19" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
       <c r="I19" s="11"/>
@@ -6475,7 +6475,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD19" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE19" s="19"/>
@@ -6483,11 +6483,11 @@
         <v>39</v>
       </c>
       <c r="AG19" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE19,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH19" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF19,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6502,7 +6502,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="20"/>
       <c r="H20" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="I20" s="11"/>
@@ -6551,7 +6551,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD20" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE20" s="19"/>
@@ -6559,11 +6559,11 @@
         <v>39</v>
       </c>
       <c r="AG20" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE20,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH20" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF20,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6578,7 +6578,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="20"/>
       <c r="H21" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>19</v>
       </c>
       <c r="I21" s="11"/>
@@ -6627,7 +6627,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD21" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE21" s="19"/>
@@ -6635,11 +6635,11 @@
         <v>39</v>
       </c>
       <c r="AG21" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE21,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH21" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF21,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6654,7 +6654,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="20"/>
       <c r="H22" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="I22" s="11"/>
@@ -6703,7 +6703,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD22" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE22" s="19"/>
@@ -6711,11 +6711,11 @@
         <v>39</v>
       </c>
       <c r="AG22" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE22,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH22" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF22,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6730,7 +6730,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="20"/>
       <c r="H23" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="I23" s="11"/>
@@ -6779,7 +6779,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD23" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE23" s="19"/>
@@ -6787,11 +6787,11 @@
         <v>39</v>
       </c>
       <c r="AG23" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE23,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH23" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF23,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6806,7 +6806,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="20"/>
       <c r="H24" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
       <c r="I24" s="11"/>
@@ -6855,7 +6855,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD24" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE24" s="19"/>
@@ -6863,11 +6863,11 @@
         <v>39</v>
       </c>
       <c r="AG24" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE24,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH24" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF24,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6882,7 +6882,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="20"/>
       <c r="H25" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23</v>
       </c>
       <c r="I25" s="11"/>
@@ -6931,7 +6931,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD25" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE25" s="19"/>
@@ -6939,11 +6939,11 @@
         <v>39</v>
       </c>
       <c r="AG25" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE25,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH25" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF25,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6958,7 +6958,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="20"/>
       <c r="H26" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="I26" s="11"/>
@@ -7007,7 +7007,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD26" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE26" s="19"/>
@@ -7015,11 +7015,11 @@
         <v>39</v>
       </c>
       <c r="AG26" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE26,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH26" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF26,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7034,7 +7034,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="20"/>
       <c r="H27" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
       <c r="I27" s="11"/>
@@ -7083,7 +7083,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD27" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE27" s="19"/>
@@ -7091,11 +7091,11 @@
         <v>39</v>
       </c>
       <c r="AG27" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE27,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH27" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF27,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7110,7 +7110,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="20"/>
       <c r="H28" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="I28" s="11"/>
@@ -7159,7 +7159,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD28" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE28" s="19"/>
@@ -7167,11 +7167,11 @@
         <v>39</v>
       </c>
       <c r="AG28" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE28,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH28" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF28,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7186,7 +7186,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="20"/>
       <c r="H29" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
       <c r="I29" s="11"/>
@@ -7235,7 +7235,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD29" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE29" s="19"/>
@@ -7243,11 +7243,11 @@
         <v>39</v>
       </c>
       <c r="AG29" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE29,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH29" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF29,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7262,7 +7262,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="20"/>
       <c r="H30" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="I30" s="11"/>
@@ -7311,7 +7311,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD30" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE30" s="19"/>
@@ -7319,11 +7319,11 @@
         <v>39</v>
       </c>
       <c r="AG30" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE30,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH30" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF30,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7338,7 +7338,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="20"/>
       <c r="H31" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>29</v>
       </c>
       <c r="I31" s="11"/>
@@ -7387,7 +7387,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD31" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE31" s="19"/>
@@ -7395,11 +7395,11 @@
         <v>39</v>
       </c>
       <c r="AG31" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE31,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH31" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF31,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7414,7 +7414,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="20"/>
       <c r="H32" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="I32" s="11"/>
@@ -7463,7 +7463,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD32" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE32" s="19"/>
@@ -7471,11 +7471,11 @@
         <v>39</v>
       </c>
       <c r="AG32" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE32,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH32" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF32,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7490,7 +7490,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="20"/>
       <c r="H33" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="I33" s="11"/>
@@ -7539,7 +7539,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD33" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE33" s="19"/>
@@ -7547,11 +7547,11 @@
         <v>39</v>
       </c>
       <c r="AG33" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE33,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH33" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF33,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7566,7 +7566,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="20"/>
       <c r="H34" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="I34" s="11"/>
@@ -7615,7 +7615,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD34" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE34" s="19"/>
@@ -7623,11 +7623,11 @@
         <v>39</v>
       </c>
       <c r="AG34" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE34,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH34" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF34,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7642,7 +7642,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="20"/>
       <c r="H35" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>33</v>
       </c>
       <c r="I35" s="11"/>
@@ -7691,7 +7691,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD35" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE35" s="19"/>
@@ -7699,11 +7699,11 @@
         <v>39</v>
       </c>
       <c r="AG35" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE35,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH35" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF35,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7718,7 +7718,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="20"/>
       <c r="H36" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>34</v>
       </c>
       <c r="I36" s="11"/>
@@ -7767,7 +7767,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD36" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE36" s="19"/>
@@ -7775,11 +7775,11 @@
         <v>39</v>
       </c>
       <c r="AG36" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE36,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH36" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF36,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7794,7 +7794,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="20"/>
       <c r="H37" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
       <c r="I37" s="11"/>
@@ -7843,7 +7843,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD37" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE37" s="19"/>
@@ -7851,11 +7851,11 @@
         <v>39</v>
       </c>
       <c r="AG37" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE37,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH37" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF37,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7870,7 +7870,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="20"/>
       <c r="H38" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
       <c r="I38" s="11"/>
@@ -7919,7 +7919,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD38" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE38" s="19"/>
@@ -7927,11 +7927,11 @@
         <v>39</v>
       </c>
       <c r="AG38" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE38,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH38" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF38,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7946,7 +7946,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="20"/>
       <c r="H39" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>37</v>
       </c>
       <c r="I39" s="11"/>
@@ -7995,7 +7995,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD39" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE39" s="19"/>
@@ -8003,11 +8003,11 @@
         <v>39</v>
       </c>
       <c r="AG39" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE39,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH39" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF39,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8022,7 +8022,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="20"/>
       <c r="H40" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
       <c r="I40" s="11"/>
@@ -8071,7 +8071,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD40" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE40" s="19"/>
@@ -8079,11 +8079,11 @@
         <v>39</v>
       </c>
       <c r="AG40" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE40,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH40" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF40,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8098,7 +8098,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="20"/>
       <c r="H41" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>39</v>
       </c>
       <c r="I41" s="11"/>
@@ -8147,7 +8147,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD41" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE41" s="19"/>
@@ -8155,11 +8155,11 @@
         <v>39</v>
       </c>
       <c r="AG41" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE41,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH41" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF41,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8174,7 +8174,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="20"/>
       <c r="H42" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="I42" s="11"/>
@@ -8223,7 +8223,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD42" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE42" s="19"/>
@@ -8231,11 +8231,11 @@
         <v>39</v>
       </c>
       <c r="AG42" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE42,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH42" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF42,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8250,7 +8250,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="20"/>
       <c r="H43" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>41</v>
       </c>
       <c r="I43" s="11"/>
@@ -8299,7 +8299,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD43" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE43" s="19"/>
@@ -8307,11 +8307,11 @@
         <v>39</v>
       </c>
       <c r="AG43" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE43,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH43" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF43,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8326,7 +8326,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="20"/>
       <c r="H44" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>42</v>
       </c>
       <c r="I44" s="11"/>
@@ -8375,7 +8375,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD44" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE44" s="19"/>
@@ -8383,11 +8383,11 @@
         <v>39</v>
       </c>
       <c r="AG44" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE44,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH44" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF44,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8402,7 +8402,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="20"/>
       <c r="H45" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>43</v>
       </c>
       <c r="I45" s="11"/>
@@ -8451,7 +8451,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD45" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE45" s="19"/>
@@ -8459,11 +8459,11 @@
         <v>39</v>
       </c>
       <c r="AG45" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE45,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH45" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF45,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8478,7 +8478,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="20"/>
       <c r="H46" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44</v>
       </c>
       <c r="I46" s="11"/>
@@ -8527,7 +8527,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD46" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE46" s="19"/>
@@ -8535,11 +8535,11 @@
         <v>39</v>
       </c>
       <c r="AG46" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE46,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH46" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF46,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8554,7 +8554,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="20"/>
       <c r="H47" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="I47" s="11"/>
@@ -8603,7 +8603,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD47" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE47" s="19"/>
@@ -8611,11 +8611,11 @@
         <v>39</v>
       </c>
       <c r="AG47" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE47,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH47" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF47,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8630,7 +8630,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="20"/>
       <c r="H48" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>46</v>
       </c>
       <c r="I48" s="11"/>
@@ -8679,7 +8679,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD48" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE48" s="19"/>
@@ -8687,11 +8687,11 @@
         <v>39</v>
       </c>
       <c r="AG48" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE48,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH48" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF48,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8706,7 +8706,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="20"/>
       <c r="H49" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>47</v>
       </c>
       <c r="I49" s="11"/>
@@ -8755,7 +8755,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD49" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE49" s="19"/>
@@ -8763,11 +8763,11 @@
         <v>39</v>
       </c>
       <c r="AG49" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE49,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH49" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF49,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8782,7 +8782,7 @@
       <c r="F50" s="22"/>
       <c r="G50" s="23"/>
       <c r="H50" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
       <c r="I50" s="22"/>
@@ -8831,7 +8831,7 @@
         <v>#N/A</v>
       </c>
       <c r="AD50" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE50" s="21"/>
@@ -8839,11 +8839,11 @@
         <v>39</v>
       </c>
       <c r="AG50" s="25" t="e">
-        <f>INDEX(ProductionListVnum, MATCH(AE50,ProductionList,0), 1)</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AH50" s="11">
-        <f>INDEX(KnowledgeVnum, MATCH(AF50,Knowledge,0), 2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -8852,16 +8852,16 @@
     <sortCondition ref="A3:A12"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
     <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AG1:AH1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J50 C3:C50">
@@ -9879,8 +9879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView topLeftCell="H91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T100" sqref="T100"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add natural weapon attack to body parts
</commit_message>
<xml_diff>
--- a/doc/RadMudEditor.xlsx
+++ b/doc/RadMudEditor.xlsx
@@ -9,15 +9,16 @@
   <sheets>
     <sheet name="RaceBaseSkill" sheetId="8" r:id="rId1"/>
     <sheet name="RaceBaseAbility" sheetId="9" r:id="rId2"/>
-    <sheet name="SkillManager" sheetId="7" r:id="rId3"/>
-    <sheet name="SkillPrerequisites" sheetId="10" r:id="rId4"/>
-    <sheet name="BodyPartResources" sheetId="14" r:id="rId5"/>
-    <sheet name="BodyPart" sheetId="12" r:id="rId6"/>
-    <sheet name="Material" sheetId="11" r:id="rId7"/>
-    <sheet name="Model" sheetId="13" r:id="rId8"/>
-    <sheet name="Variables" sheetId="6" r:id="rId9"/>
-    <sheet name="Profession" sheetId="17" r:id="rId10"/>
-    <sheet name="Production" sheetId="16" r:id="rId11"/>
+    <sheet name="RaceNaturalWeapon" sheetId="18" r:id="rId3"/>
+    <sheet name="SkillManager" sheetId="7" r:id="rId4"/>
+    <sheet name="SkillPrerequisites" sheetId="10" r:id="rId5"/>
+    <sheet name="BodyPartResources" sheetId="14" r:id="rId6"/>
+    <sheet name="BodyPart" sheetId="12" r:id="rId7"/>
+    <sheet name="Material" sheetId="11" r:id="rId8"/>
+    <sheet name="Model" sheetId="13" r:id="rId9"/>
+    <sheet name="Variables" sheetId="6" r:id="rId10"/>
+    <sheet name="Profession" sheetId="17" r:id="rId11"/>
+    <sheet name="Production" sheetId="16" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Ability">Variables!$C$2:$C$6</definedName>
@@ -2068,6 +2069,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2075,15 +2085,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2402,9 +2403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4099,10 +4098,1522 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="9">
+        <v>0</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="P3" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="R3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="9">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="9">
+        <v>2</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="9">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>2</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="9">
+        <v>2</v>
+      </c>
+      <c r="P4" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="R4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>4</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="9">
+        <v>3</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="9">
+        <v>3</v>
+      </c>
+      <c r="P5" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="R5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="9">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4</v>
+      </c>
+      <c r="J6" s="9">
+        <v>4</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="9">
+        <v>4</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="9">
+        <v>4</v>
+      </c>
+      <c r="P6" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="R6" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="9">
+        <v>6</v>
+      </c>
+      <c r="H7" s="9">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9">
+        <v>5</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="9">
+        <v>5</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="9">
+        <v>5</v>
+      </c>
+      <c r="P7" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="R7" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="9">
+        <v>7</v>
+      </c>
+      <c r="H8" s="9">
+        <v>6</v>
+      </c>
+      <c r="J8" s="9">
+        <v>6</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="9">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="9">
+        <v>6</v>
+      </c>
+      <c r="P8" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="R8" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="9">
+        <v>7</v>
+      </c>
+      <c r="J9" s="9">
+        <v>7</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="9">
+        <v>7</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="9">
+        <v>7</v>
+      </c>
+      <c r="P9" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="R9" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9">
+        <v>8</v>
+      </c>
+      <c r="J10" s="9">
+        <v>8</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="9">
+        <v>8</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="9">
+        <v>8</v>
+      </c>
+      <c r="P10" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="R10" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9">
+        <v>10</v>
+      </c>
+      <c r="H11" s="9">
+        <v>9</v>
+      </c>
+      <c r="J11" s="9">
+        <v>9</v>
+      </c>
+      <c r="L11" s="9">
+        <v>9</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="9">
+        <v>9</v>
+      </c>
+      <c r="P11" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="R11" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>11</v>
+      </c>
+      <c r="H12" s="9">
+        <v>10</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="9">
+        <v>10</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="9">
+        <v>10</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="9">
+        <v>10</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="P12" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="R12" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="9">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9">
+        <v>11</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="9">
+        <v>11</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="9">
+        <v>11</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="9">
+        <v>11</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="P13" s="9">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R13" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="9">
+        <v>13</v>
+      </c>
+      <c r="H14" s="9">
+        <v>12</v>
+      </c>
+      <c r="J14" s="9">
+        <v>12</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="9">
+        <v>12</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="9">
+        <v>12</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="P14" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="R14" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9">
+        <v>14</v>
+      </c>
+      <c r="H15" s="9">
+        <v>13</v>
+      </c>
+      <c r="J15" s="9">
+        <v>13</v>
+      </c>
+      <c r="L15" s="9">
+        <v>13</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N15" s="9">
+        <v>13</v>
+      </c>
+      <c r="P15" s="9">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="R15" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="9">
+        <v>15</v>
+      </c>
+      <c r="H16" s="9">
+        <v>14</v>
+      </c>
+      <c r="J16" s="9">
+        <v>14</v>
+      </c>
+      <c r="L16" s="9">
+        <v>14</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="9">
+        <v>14</v>
+      </c>
+      <c r="P16" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="R16" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9">
+        <v>16</v>
+      </c>
+      <c r="H17" s="9">
+        <v>15</v>
+      </c>
+      <c r="J17" s="9">
+        <v>15</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" s="9">
+        <v>15</v>
+      </c>
+      <c r="P17" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="R17" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="9">
+        <v>17</v>
+      </c>
+      <c r="H18" s="9">
+        <v>16</v>
+      </c>
+      <c r="J18" s="9">
+        <v>16</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" s="9">
+        <v>16</v>
+      </c>
+      <c r="P18" s="9">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="R18" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="9">
+        <v>18</v>
+      </c>
+      <c r="H19" s="9">
+        <v>17</v>
+      </c>
+      <c r="J19" s="9">
+        <v>17</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="L19" s="9">
+        <v>17</v>
+      </c>
+      <c r="P19" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="R19" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="9">
+        <v>19</v>
+      </c>
+      <c r="H20" s="9">
+        <v>18</v>
+      </c>
+      <c r="J20" s="9">
+        <v>18</v>
+      </c>
+      <c r="L20" s="9">
+        <v>18</v>
+      </c>
+      <c r="P20" s="9">
+        <v>18</v>
+      </c>
+      <c r="R20" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="9">
+        <v>20</v>
+      </c>
+      <c r="H21" s="9">
+        <v>19</v>
+      </c>
+      <c r="J21" s="9">
+        <v>19</v>
+      </c>
+      <c r="L21" s="9">
+        <v>19</v>
+      </c>
+      <c r="P21" s="9">
+        <v>19</v>
+      </c>
+      <c r="R21" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="9">
+        <v>21</v>
+      </c>
+      <c r="H22" s="9">
+        <v>20</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="9">
+        <v>20</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="9">
+        <v>20</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="P22" s="9">
+        <v>20</v>
+      </c>
+      <c r="R22" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9">
+        <v>22</v>
+      </c>
+      <c r="H23" s="9">
+        <v>21</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="9">
+        <v>21</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="9">
+        <v>21</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="P23" s="9">
+        <v>21</v>
+      </c>
+      <c r="R23" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="9">
+        <v>23</v>
+      </c>
+      <c r="H24" s="9">
+        <v>22</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J24" s="9">
+        <v>22</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L24" s="9">
+        <v>22</v>
+      </c>
+      <c r="P24" s="9">
+        <v>22</v>
+      </c>
+      <c r="R24" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="9">
+        <v>24</v>
+      </c>
+      <c r="H25" s="9">
+        <v>23</v>
+      </c>
+      <c r="J25" s="9">
+        <v>23</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="L25" s="9">
+        <v>23</v>
+      </c>
+      <c r="P25" s="9">
+        <v>23</v>
+      </c>
+      <c r="R25" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="9">
+        <v>25</v>
+      </c>
+      <c r="H26" s="9">
+        <v>24</v>
+      </c>
+      <c r="J26" s="9">
+        <v>24</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L26" s="9">
+        <v>24</v>
+      </c>
+      <c r="P26" s="9">
+        <v>24</v>
+      </c>
+      <c r="R26" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="9">
+        <v>26</v>
+      </c>
+      <c r="H27" s="9">
+        <v>25</v>
+      </c>
+      <c r="J27" s="9">
+        <v>25</v>
+      </c>
+      <c r="L27" s="9">
+        <v>25</v>
+      </c>
+      <c r="P27" s="9">
+        <v>25</v>
+      </c>
+      <c r="R27" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="9">
+        <v>27</v>
+      </c>
+      <c r="J28" s="9">
+        <v>26</v>
+      </c>
+      <c r="L28" s="9">
+        <v>26</v>
+      </c>
+      <c r="P28" s="9">
+        <v>26</v>
+      </c>
+      <c r="R28" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="9">
+        <v>28</v>
+      </c>
+      <c r="J29" s="9">
+        <v>27</v>
+      </c>
+      <c r="L29" s="9">
+        <v>27</v>
+      </c>
+      <c r="P29" s="9">
+        <v>27</v>
+      </c>
+      <c r="R29" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="9">
+        <v>29</v>
+      </c>
+      <c r="J30" s="9">
+        <v>28</v>
+      </c>
+      <c r="L30" s="9">
+        <v>28</v>
+      </c>
+      <c r="P30" s="9">
+        <v>28</v>
+      </c>
+      <c r="R30" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="9">
+        <v>30</v>
+      </c>
+      <c r="J31" s="9">
+        <v>29</v>
+      </c>
+      <c r="L31" s="9">
+        <v>29</v>
+      </c>
+      <c r="P31" s="9">
+        <v>29</v>
+      </c>
+      <c r="R31" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="9">
+        <v>31</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="9">
+        <v>30</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L32" s="9">
+        <v>30</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="P32" s="9">
+        <v>30</v>
+      </c>
+      <c r="R32" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="9">
+        <v>32</v>
+      </c>
+      <c r="J33" s="9">
+        <v>31</v>
+      </c>
+      <c r="L33" s="9">
+        <v>31</v>
+      </c>
+      <c r="O33" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="P33" s="9">
+        <v>31</v>
+      </c>
+      <c r="R33" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E34" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="9">
+        <v>33</v>
+      </c>
+      <c r="J34" s="9">
+        <v>32</v>
+      </c>
+      <c r="L34" s="9">
+        <v>32</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="P34" s="9">
+        <v>32</v>
+      </c>
+      <c r="R34" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="9">
+        <v>34</v>
+      </c>
+      <c r="J35" s="9">
+        <v>33</v>
+      </c>
+      <c r="L35" s="9">
+        <v>33</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="P35" s="9">
+        <v>33</v>
+      </c>
+      <c r="R35" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E36" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="9">
+        <v>35</v>
+      </c>
+      <c r="J36" s="9">
+        <v>34</v>
+      </c>
+      <c r="L36" s="9">
+        <v>34</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="P36" s="9">
+        <v>34</v>
+      </c>
+      <c r="R36" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E37" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" s="9">
+        <v>36</v>
+      </c>
+      <c r="J37" s="9">
+        <v>35</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L37" s="9">
+        <v>35</v>
+      </c>
+      <c r="P37" s="9">
+        <v>35</v>
+      </c>
+      <c r="R37" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E38" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="9">
+        <v>37</v>
+      </c>
+      <c r="J38" s="9">
+        <v>36</v>
+      </c>
+      <c r="L38" s="9">
+        <v>36</v>
+      </c>
+      <c r="P38" s="9">
+        <v>36</v>
+      </c>
+      <c r="R38" s="9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E39" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="9">
+        <v>38</v>
+      </c>
+      <c r="J39" s="9">
+        <v>37</v>
+      </c>
+      <c r="L39" s="9">
+        <v>37</v>
+      </c>
+      <c r="P39" s="9">
+        <v>37</v>
+      </c>
+      <c r="R39" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E40" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="9">
+        <v>39</v>
+      </c>
+      <c r="J40" s="9">
+        <v>38</v>
+      </c>
+      <c r="L40" s="9">
+        <v>38</v>
+      </c>
+      <c r="P40" s="9">
+        <v>38</v>
+      </c>
+      <c r="R40" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E41" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="9">
+        <v>40</v>
+      </c>
+      <c r="J41" s="9">
+        <v>39</v>
+      </c>
+      <c r="L41" s="9">
+        <v>39</v>
+      </c>
+      <c r="P41" s="9">
+        <v>39</v>
+      </c>
+      <c r="R41" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E42" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="9">
+        <v>41</v>
+      </c>
+      <c r="J42" s="9">
+        <v>40</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="L42" s="9">
+        <v>40</v>
+      </c>
+      <c r="O42" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="P42" s="9">
+        <v>40</v>
+      </c>
+      <c r="R42" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E43" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="9">
+        <v>42</v>
+      </c>
+      <c r="J43" s="9">
+        <v>41</v>
+      </c>
+      <c r="L43" s="9">
+        <v>41</v>
+      </c>
+      <c r="P43" s="9">
+        <v>41</v>
+      </c>
+      <c r="R43" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="F44" s="9">
+        <v>43</v>
+      </c>
+      <c r="J44" s="9">
+        <v>42</v>
+      </c>
+      <c r="L44" s="9">
+        <v>42</v>
+      </c>
+      <c r="P44" s="9">
+        <v>42</v>
+      </c>
+      <c r="R44" s="9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="F45" s="9">
+        <v>44</v>
+      </c>
+      <c r="J45" s="9">
+        <v>43</v>
+      </c>
+      <c r="L45" s="9">
+        <v>43</v>
+      </c>
+      <c r="P45" s="9">
+        <v>43</v>
+      </c>
+      <c r="R45" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="F46" s="9">
+        <v>45</v>
+      </c>
+      <c r="J46" s="9">
+        <v>44</v>
+      </c>
+      <c r="L46" s="9">
+        <v>44</v>
+      </c>
+      <c r="P46" s="9">
+        <v>44</v>
+      </c>
+      <c r="R46" s="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="F47" s="9">
+        <v>46</v>
+      </c>
+      <c r="J47" s="9">
+        <v>45</v>
+      </c>
+      <c r="L47" s="9">
+        <v>45</v>
+      </c>
+      <c r="P47" s="9">
+        <v>45</v>
+      </c>
+      <c r="R47" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="F48" s="9">
+        <v>47</v>
+      </c>
+      <c r="J48" s="9">
+        <v>46</v>
+      </c>
+      <c r="L48" s="9">
+        <v>46</v>
+      </c>
+      <c r="P48" s="9">
+        <v>46</v>
+      </c>
+      <c r="R48" s="9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F49" s="9">
+        <v>48</v>
+      </c>
+      <c r="J49" s="9">
+        <v>47</v>
+      </c>
+      <c r="L49" s="9">
+        <v>47</v>
+      </c>
+      <c r="P49" s="9">
+        <v>47</v>
+      </c>
+      <c r="R49" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F50" s="9">
+        <v>49</v>
+      </c>
+      <c r="J50" s="9">
+        <v>48</v>
+      </c>
+      <c r="L50" s="9">
+        <v>48</v>
+      </c>
+      <c r="P50" s="9">
+        <v>48</v>
+      </c>
+      <c r="R50" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F51" s="9">
+        <v>50</v>
+      </c>
+      <c r="J51" s="9">
+        <v>49</v>
+      </c>
+      <c r="L51" s="9">
+        <v>49</v>
+      </c>
+      <c r="P51" s="9">
+        <v>49</v>
+      </c>
+      <c r="R51" s="9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F52" s="9">
+        <v>51</v>
+      </c>
+      <c r="J52" s="9">
+        <v>50</v>
+      </c>
+      <c r="L52" s="9">
+        <v>50</v>
+      </c>
+      <c r="P52" s="9">
+        <v>50</v>
+      </c>
+      <c r="R52" s="9">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
@@ -4586,7 +6097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH50"/>
   <sheetViews>
@@ -4632,60 +6143,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="36" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="33" t="s">
         <v>555</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="36" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="33" t="s">
         <v>556</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="36" t="s">
+      <c r="P1" s="34"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="33" t="s">
         <v>556</v>
       </c>
-      <c r="S1" s="37"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="36" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="33" t="s">
         <v>557</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="36" t="s">
+      <c r="V1" s="35"/>
+      <c r="W1" s="33" t="s">
         <v>557</v>
       </c>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="36" t="s">
+      <c r="X1" s="35"/>
+      <c r="Y1" s="33" t="s">
         <v>558</v>
       </c>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="33" t="s">
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="36" t="s">
         <v>558</v>
       </c>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="36" t="s">
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="36" t="s">
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="37"/>
+      <c r="AH1" s="34"/>
     </row>
     <row r="2" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -9877,9 +11388,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -14744,7 +16267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D105"/>
   <sheetViews>
@@ -16070,12 +17593,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17956,7 +19479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -18325,7 +19848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
@@ -19604,7 +21127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O52"/>
   <sheetViews>
@@ -22028,1515 +23551,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>559</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="9">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="P3" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="R3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="9">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="9">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="9">
-        <v>3</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="9">
-        <v>2</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="9">
-        <v>2</v>
-      </c>
-      <c r="L4" s="9">
-        <v>2</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="9">
-        <v>2</v>
-      </c>
-      <c r="P4" s="9">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="R4" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="9">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="9">
-        <v>4</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
-        <v>4</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="9">
-        <v>3</v>
-      </c>
-      <c r="J5" s="9">
-        <v>3</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="L5" s="9">
-        <v>3</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" s="9">
-        <v>3</v>
-      </c>
-      <c r="P5" s="9">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="R5" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="9">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="9">
-        <v>5</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="9">
-        <v>5</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="9">
-        <v>4</v>
-      </c>
-      <c r="J6" s="9">
-        <v>4</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="9">
-        <v>4</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="9">
-        <v>4</v>
-      </c>
-      <c r="P6" s="9">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="R6" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="9">
-        <v>6</v>
-      </c>
-      <c r="H7" s="9">
-        <v>5</v>
-      </c>
-      <c r="J7" s="9">
-        <v>5</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" s="9">
-        <v>5</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" s="9">
-        <v>5</v>
-      </c>
-      <c r="P7" s="9">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>563</v>
-      </c>
-      <c r="R7" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E8" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="9">
-        <v>7</v>
-      </c>
-      <c r="H8" s="9">
-        <v>6</v>
-      </c>
-      <c r="J8" s="9">
-        <v>6</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="9">
-        <v>6</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="9">
-        <v>6</v>
-      </c>
-      <c r="P8" s="9">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="R8" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="9">
-        <v>8</v>
-      </c>
-      <c r="H9" s="9">
-        <v>7</v>
-      </c>
-      <c r="J9" s="9">
-        <v>7</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="9">
-        <v>7</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="9">
-        <v>7</v>
-      </c>
-      <c r="P9" s="9">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>565</v>
-      </c>
-      <c r="R9" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>9</v>
-      </c>
-      <c r="H10" s="9">
-        <v>8</v>
-      </c>
-      <c r="J10" s="9">
-        <v>8</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" s="9">
-        <v>8</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="9">
-        <v>8</v>
-      </c>
-      <c r="P10" s="9">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="R10" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="9">
-        <v>10</v>
-      </c>
-      <c r="H11" s="9">
-        <v>9</v>
-      </c>
-      <c r="J11" s="9">
-        <v>9</v>
-      </c>
-      <c r="L11" s="9">
-        <v>9</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="N11" s="9">
-        <v>9</v>
-      </c>
-      <c r="P11" s="9">
-        <v>9</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>567</v>
-      </c>
-      <c r="R11" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>11</v>
-      </c>
-      <c r="H12" s="9">
-        <v>10</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" s="9">
-        <v>10</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" s="9">
-        <v>10</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="9">
-        <v>10</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="P12" s="9">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>568</v>
-      </c>
-      <c r="R12" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E13" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="9">
-        <v>12</v>
-      </c>
-      <c r="H13" s="9">
-        <v>11</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="9">
-        <v>11</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" s="9">
-        <v>11</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="N13" s="9">
-        <v>11</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="P13" s="9">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>569</v>
-      </c>
-      <c r="R13" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="9">
-        <v>13</v>
-      </c>
-      <c r="H14" s="9">
-        <v>12</v>
-      </c>
-      <c r="J14" s="9">
-        <v>12</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L14" s="9">
-        <v>12</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="N14" s="9">
-        <v>12</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="P14" s="9">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="R14" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="9">
-        <v>14</v>
-      </c>
-      <c r="H15" s="9">
-        <v>13</v>
-      </c>
-      <c r="J15" s="9">
-        <v>13</v>
-      </c>
-      <c r="L15" s="9">
-        <v>13</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="N15" s="9">
-        <v>13</v>
-      </c>
-      <c r="P15" s="9">
-        <v>13</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="R15" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="9">
-        <v>15</v>
-      </c>
-      <c r="H16" s="9">
-        <v>14</v>
-      </c>
-      <c r="J16" s="9">
-        <v>14</v>
-      </c>
-      <c r="L16" s="9">
-        <v>14</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" s="9">
-        <v>14</v>
-      </c>
-      <c r="P16" s="9">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>572</v>
-      </c>
-      <c r="R16" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="9">
-        <v>16</v>
-      </c>
-      <c r="H17" s="9">
-        <v>15</v>
-      </c>
-      <c r="J17" s="9">
-        <v>15</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L17" s="9">
-        <v>15</v>
-      </c>
-      <c r="P17" s="9">
-        <v>15</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="R17" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="9">
-        <v>17</v>
-      </c>
-      <c r="H18" s="9">
-        <v>16</v>
-      </c>
-      <c r="J18" s="9">
-        <v>16</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="L18" s="9">
-        <v>16</v>
-      </c>
-      <c r="P18" s="9">
-        <v>16</v>
-      </c>
-      <c r="Q18" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="R18" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="9">
-        <v>18</v>
-      </c>
-      <c r="H19" s="9">
-        <v>17</v>
-      </c>
-      <c r="J19" s="9">
-        <v>17</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="L19" s="9">
-        <v>17</v>
-      </c>
-      <c r="P19" s="9">
-        <v>17</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>573</v>
-      </c>
-      <c r="R19" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="9">
-        <v>19</v>
-      </c>
-      <c r="H20" s="9">
-        <v>18</v>
-      </c>
-      <c r="J20" s="9">
-        <v>18</v>
-      </c>
-      <c r="L20" s="9">
-        <v>18</v>
-      </c>
-      <c r="P20" s="9">
-        <v>18</v>
-      </c>
-      <c r="R20" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="9">
-        <v>20</v>
-      </c>
-      <c r="H21" s="9">
-        <v>19</v>
-      </c>
-      <c r="J21" s="9">
-        <v>19</v>
-      </c>
-      <c r="L21" s="9">
-        <v>19</v>
-      </c>
-      <c r="P21" s="9">
-        <v>19</v>
-      </c>
-      <c r="R21" s="9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="9">
-        <v>21</v>
-      </c>
-      <c r="H22" s="9">
-        <v>20</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="9">
-        <v>20</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L22" s="9">
-        <v>20</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="P22" s="9">
-        <v>20</v>
-      </c>
-      <c r="R22" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="9">
-        <v>22</v>
-      </c>
-      <c r="H23" s="9">
-        <v>21</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="9">
-        <v>21</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="L23" s="9">
-        <v>21</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="P23" s="9">
-        <v>21</v>
-      </c>
-      <c r="R23" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="9">
-        <v>23</v>
-      </c>
-      <c r="H24" s="9">
-        <v>22</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="9">
-        <v>22</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" s="9">
-        <v>22</v>
-      </c>
-      <c r="P24" s="9">
-        <v>22</v>
-      </c>
-      <c r="R24" s="9">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="9">
-        <v>24</v>
-      </c>
-      <c r="H25" s="9">
-        <v>23</v>
-      </c>
-      <c r="J25" s="9">
-        <v>23</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="L25" s="9">
-        <v>23</v>
-      </c>
-      <c r="P25" s="9">
-        <v>23</v>
-      </c>
-      <c r="R25" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E26" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="9">
-        <v>25</v>
-      </c>
-      <c r="H26" s="9">
-        <v>24</v>
-      </c>
-      <c r="J26" s="9">
-        <v>24</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="L26" s="9">
-        <v>24</v>
-      </c>
-      <c r="P26" s="9">
-        <v>24</v>
-      </c>
-      <c r="R26" s="9">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E27" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="9">
-        <v>26</v>
-      </c>
-      <c r="H27" s="9">
-        <v>25</v>
-      </c>
-      <c r="J27" s="9">
-        <v>25</v>
-      </c>
-      <c r="L27" s="9">
-        <v>25</v>
-      </c>
-      <c r="P27" s="9">
-        <v>25</v>
-      </c>
-      <c r="R27" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E28" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="9">
-        <v>27</v>
-      </c>
-      <c r="J28" s="9">
-        <v>26</v>
-      </c>
-      <c r="L28" s="9">
-        <v>26</v>
-      </c>
-      <c r="P28" s="9">
-        <v>26</v>
-      </c>
-      <c r="R28" s="9">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="9">
-        <v>28</v>
-      </c>
-      <c r="J29" s="9">
-        <v>27</v>
-      </c>
-      <c r="L29" s="9">
-        <v>27</v>
-      </c>
-      <c r="P29" s="9">
-        <v>27</v>
-      </c>
-      <c r="R29" s="9">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E30" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="9">
-        <v>29</v>
-      </c>
-      <c r="J30" s="9">
-        <v>28</v>
-      </c>
-      <c r="L30" s="9">
-        <v>28</v>
-      </c>
-      <c r="P30" s="9">
-        <v>28</v>
-      </c>
-      <c r="R30" s="9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="9">
-        <v>30</v>
-      </c>
-      <c r="J31" s="9">
-        <v>29</v>
-      </c>
-      <c r="L31" s="9">
-        <v>29</v>
-      </c>
-      <c r="P31" s="9">
-        <v>29</v>
-      </c>
-      <c r="R31" s="9">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E32" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="9">
-        <v>31</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J32" s="9">
-        <v>30</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="L32" s="9">
-        <v>30</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="P32" s="9">
-        <v>30</v>
-      </c>
-      <c r="R32" s="9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E33" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="9">
-        <v>32</v>
-      </c>
-      <c r="J33" s="9">
-        <v>31</v>
-      </c>
-      <c r="L33" s="9">
-        <v>31</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="P33" s="9">
-        <v>31</v>
-      </c>
-      <c r="R33" s="9">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E34" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="9">
-        <v>33</v>
-      </c>
-      <c r="J34" s="9">
-        <v>32</v>
-      </c>
-      <c r="L34" s="9">
-        <v>32</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="P34" s="9">
-        <v>32</v>
-      </c>
-      <c r="R34" s="9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E35" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="9">
-        <v>34</v>
-      </c>
-      <c r="J35" s="9">
-        <v>33</v>
-      </c>
-      <c r="L35" s="9">
-        <v>33</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="P35" s="9">
-        <v>33</v>
-      </c>
-      <c r="R35" s="9">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E36" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="9">
-        <v>35</v>
-      </c>
-      <c r="J36" s="9">
-        <v>34</v>
-      </c>
-      <c r="L36" s="9">
-        <v>34</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="P36" s="9">
-        <v>34</v>
-      </c>
-      <c r="R36" s="9">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E37" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F37" s="9">
-        <v>36</v>
-      </c>
-      <c r="J37" s="9">
-        <v>35</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="L37" s="9">
-        <v>35</v>
-      </c>
-      <c r="P37" s="9">
-        <v>35</v>
-      </c>
-      <c r="R37" s="9">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E38" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" s="9">
-        <v>37</v>
-      </c>
-      <c r="J38" s="9">
-        <v>36</v>
-      </c>
-      <c r="L38" s="9">
-        <v>36</v>
-      </c>
-      <c r="P38" s="9">
-        <v>36</v>
-      </c>
-      <c r="R38" s="9">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E39" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F39" s="9">
-        <v>38</v>
-      </c>
-      <c r="J39" s="9">
-        <v>37</v>
-      </c>
-      <c r="L39" s="9">
-        <v>37</v>
-      </c>
-      <c r="P39" s="9">
-        <v>37</v>
-      </c>
-      <c r="R39" s="9">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" s="9">
-        <v>39</v>
-      </c>
-      <c r="J40" s="9">
-        <v>38</v>
-      </c>
-      <c r="L40" s="9">
-        <v>38</v>
-      </c>
-      <c r="P40" s="9">
-        <v>38</v>
-      </c>
-      <c r="R40" s="9">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E41" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="9">
-        <v>40</v>
-      </c>
-      <c r="J41" s="9">
-        <v>39</v>
-      </c>
-      <c r="L41" s="9">
-        <v>39</v>
-      </c>
-      <c r="P41" s="9">
-        <v>39</v>
-      </c>
-      <c r="R41" s="9">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E42" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="9">
-        <v>41</v>
-      </c>
-      <c r="J42" s="9">
-        <v>40</v>
-      </c>
-      <c r="K42" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="L42" s="9">
-        <v>40</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="P42" s="9">
-        <v>40</v>
-      </c>
-      <c r="R42" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E43" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" s="9">
-        <v>42</v>
-      </c>
-      <c r="J43" s="9">
-        <v>41</v>
-      </c>
-      <c r="L43" s="9">
-        <v>41</v>
-      </c>
-      <c r="P43" s="9">
-        <v>41</v>
-      </c>
-      <c r="R43" s="9">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F44" s="9">
-        <v>43</v>
-      </c>
-      <c r="J44" s="9">
-        <v>42</v>
-      </c>
-      <c r="L44" s="9">
-        <v>42</v>
-      </c>
-      <c r="P44" s="9">
-        <v>42</v>
-      </c>
-      <c r="R44" s="9">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F45" s="9">
-        <v>44</v>
-      </c>
-      <c r="J45" s="9">
-        <v>43</v>
-      </c>
-      <c r="L45" s="9">
-        <v>43</v>
-      </c>
-      <c r="P45" s="9">
-        <v>43</v>
-      </c>
-      <c r="R45" s="9">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F46" s="9">
-        <v>45</v>
-      </c>
-      <c r="J46" s="9">
-        <v>44</v>
-      </c>
-      <c r="L46" s="9">
-        <v>44</v>
-      </c>
-      <c r="P46" s="9">
-        <v>44</v>
-      </c>
-      <c r="R46" s="9">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F47" s="9">
-        <v>46</v>
-      </c>
-      <c r="J47" s="9">
-        <v>45</v>
-      </c>
-      <c r="L47" s="9">
-        <v>45</v>
-      </c>
-      <c r="P47" s="9">
-        <v>45</v>
-      </c>
-      <c r="R47" s="9">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F48" s="9">
-        <v>47</v>
-      </c>
-      <c r="J48" s="9">
-        <v>46</v>
-      </c>
-      <c r="L48" s="9">
-        <v>46</v>
-      </c>
-      <c r="P48" s="9">
-        <v>46</v>
-      </c>
-      <c r="R48" s="9">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F49" s="9">
-        <v>48</v>
-      </c>
-      <c r="J49" s="9">
-        <v>47</v>
-      </c>
-      <c r="L49" s="9">
-        <v>47</v>
-      </c>
-      <c r="P49" s="9">
-        <v>47</v>
-      </c>
-      <c r="R49" s="9">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F50" s="9">
-        <v>49</v>
-      </c>
-      <c r="J50" s="9">
-        <v>48</v>
-      </c>
-      <c r="L50" s="9">
-        <v>48</v>
-      </c>
-      <c r="P50" s="9">
-        <v>48</v>
-      </c>
-      <c r="R50" s="9">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F51" s="9">
-        <v>50</v>
-      </c>
-      <c r="J51" s="9">
-        <v>49</v>
-      </c>
-      <c r="L51" s="9">
-        <v>49</v>
-      </c>
-      <c r="P51" s="9">
-        <v>49</v>
-      </c>
-      <c r="R51" s="9">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F52" s="9">
-        <v>51</v>
-      </c>
-      <c r="J52" s="9">
-        <v>50</v>
-      </c>
-      <c r="L52" s="9">
-        <v>50</v>
-      </c>
-      <c r="P52" s="9">
-        <v>50</v>
-      </c>
-      <c r="R52" s="9">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>